<commit_message>
update Mods for Majwara
</commit_message>
<xml_diff>
--- a/xml/OMV-MODS-worksheet.xlsx
+++ b/xml/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/onemorevoice/xml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA29DF73-25AD-EC41-A806-470FFFF3005F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FC8DA4-E292-A046-8BBD-BDCB6F16051C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="460" windowWidth="25020" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="1144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2027" uniqueCount="1152">
   <si>
     <t>liv_000017</t>
   </si>
@@ -3476,6 +3476,30 @@
   </si>
   <si>
     <t>27 August 1881</t>
+  </si>
+  <si>
+    <t>liv_020053</t>
+  </si>
+  <si>
+    <t>“Majwara's Account of the Last Journey and Death of Dr. Livingstone”</t>
+  </si>
+  <si>
+    <t>“Majwara's Account of the Last Journey and Death of Dr. Livingstone,” 13 April 1874</t>
+  </si>
+  <si>
+    <t>Majwara, c.1857-1886</t>
+  </si>
+  <si>
+    <t>Holmwood, Frederick</t>
+  </si>
+  <si>
+    <t>Proceedings of the Royal Geographical Society</t>
+  </si>
+  <si>
+    <t>244-46</t>
+  </si>
+  <si>
+    <t>12 March 1874; 13 April 1874</t>
   </si>
 </sst>
 </file>
@@ -3963,11 +3987,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AK74"/>
+  <dimension ref="A1:AK75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA46" sqref="AA46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5675,94 +5699,97 @@
         <v>892</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="187" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:37" ht="85" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>894</v>
+        <v>1144</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>895</v>
+        <v>1145</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>896</v>
+        <v>1146</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>897</v>
+        <v>1148</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>898</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>899</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>900</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>901</v>
+        <v>1147</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="AA46" s="4" t="s">
-        <v>903</v>
-      </c>
-      <c r="AB46" s="4" t="s">
-        <v>904</v>
-      </c>
-      <c r="AC46" s="4" t="s">
-        <v>905</v>
-      </c>
-      <c r="AD46" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="AH46" s="4" t="s">
-        <v>906</v>
-      </c>
-      <c r="AJ46" s="4">
-        <v>1905</v>
-      </c>
-      <c r="AK46" s="4" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="47" spans="1:37" ht="68" x14ac:dyDescent="0.2">
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="S46" s="1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="T46" s="1">
+        <v>18</v>
+      </c>
+      <c r="U46" s="1">
+        <v>3</v>
+      </c>
+      <c r="V46" s="1" t="s">
+        <v>1150</v>
+      </c>
+      <c r="W46" s="1" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="47" spans="1:37" ht="187" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>672</v>
+        <v>894</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>676</v>
+        <v>895</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>677</v>
+        <v>896</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>679</v>
+        <v>898</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>901</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>429</v>
       </c>
+      <c r="AA47" s="4" t="s">
+        <v>903</v>
+      </c>
+      <c r="AB47" s="4" t="s">
+        <v>904</v>
+      </c>
       <c r="AC47" s="4" t="s">
-        <v>681</v>
+        <v>905</v>
       </c>
       <c r="AD47" s="4" t="s">
         <v>64</v>
       </c>
       <c r="AH47" s="4" t="s">
-        <v>680</v>
+        <v>906</v>
       </c>
       <c r="AJ47" s="4">
-        <v>1904</v>
+        <v>1905</v>
       </c>
       <c r="AK47" s="4" t="s">
-        <v>682</v>
+        <v>907</v>
       </c>
     </row>
     <row r="48" spans="1:37" ht="68" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>676</v>
@@ -5792,12 +5819,12 @@
         <v>1904</v>
       </c>
       <c r="AK48" s="4" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="49" spans="1:37" ht="68" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>676</v>
@@ -5827,12 +5854,12 @@
         <v>1904</v>
       </c>
       <c r="AK49" s="4" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="50" spans="1:37" ht="68" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>676</v>
@@ -5862,107 +5889,94 @@
         <v>1904</v>
       </c>
       <c r="AK50" s="4" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="51" spans="1:37" ht="68" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="AC51" s="4" t="s">
+        <v>681</v>
+      </c>
+      <c r="AD51" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH51" s="4" t="s">
+        <v>680</v>
+      </c>
+      <c r="AJ51" s="4">
+        <v>1904</v>
+      </c>
+      <c r="AK51" s="4" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="51" spans="1:37" ht="85" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:37" ht="85" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>824</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="L51" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M51" s="7" t="s">
-        <v>611</v>
-      </c>
-      <c r="N51" s="7" t="s">
-        <v>612</v>
-      </c>
-      <c r="O51" s="1" t="s">
-        <v>828</v>
-      </c>
-      <c r="P51" s="1" t="s">
-        <v>826</v>
-      </c>
-      <c r="Q51" s="1" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="52" spans="1:37" ht="51" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>1018</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>1019</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>1020</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>1021</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="L52" s="1" t="s">
+      <c r="L52" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M52" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="N52" s="1" t="s">
-        <v>474</v>
+      <c r="M52" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="N52" s="7" t="s">
+        <v>612</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>1022</v>
+        <v>828</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>1023</v>
+        <v>826</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>1024</v>
-      </c>
-      <c r="Y52" s="1"/>
-      <c r="Z52" s="1"/>
-      <c r="AA52" s="1"/>
-      <c r="AB52" s="1"/>
-      <c r="AC52" s="1"/>
-      <c r="AD52" s="1"/>
-      <c r="AE52" s="1"/>
-      <c r="AF52" s="1"/>
-      <c r="AG52" s="1"/>
-      <c r="AH52" s="1"/>
-      <c r="AI52" s="1"/>
-      <c r="AJ52" s="1"/>
-      <c r="AK52" s="1"/>
-    </row>
-    <row r="53" spans="1:37" ht="34" x14ac:dyDescent="0.2">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="53" spans="1:37" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>1025</v>
+        <v>1018</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>1026</v>
+        <v>1019</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1027</v>
+        <v>1020</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>1028</v>
+        <v>1021</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>115</v>
@@ -5977,13 +5991,13 @@
         <v>474</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>1029</v>
+        <v>1022</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>1030</v>
+        <v>1023</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>1031</v>
+        <v>1024</v>
       </c>
       <c r="Y53" s="1"/>
       <c r="Z53" s="1"/>
@@ -6001,16 +6015,16 @@
     </row>
     <row r="54" spans="1:37" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>1032</v>
+        <v>1025</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1033</v>
+        <v>1026</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1034</v>
+        <v>1027</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1021</v>
+        <v>1028</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>115</v>
@@ -6025,13 +6039,13 @@
         <v>474</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>1035</v>
+        <v>1029</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>1036</v>
+        <v>1030</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>1037</v>
+        <v>1031</v>
       </c>
       <c r="Y54" s="1"/>
       <c r="Z54" s="1"/>
@@ -6047,18 +6061,18 @@
       <c r="AJ54" s="1"/>
       <c r="AK54" s="1"/>
     </row>
-    <row r="55" spans="1:37" ht="51" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:37" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>1038</v>
+        <v>1032</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>1039</v>
+        <v>1033</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1040</v>
+        <v>1034</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>1041</v>
+        <v>1021</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>115</v>
@@ -6073,13 +6087,13 @@
         <v>474</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>1042</v>
+        <v>1035</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>1043</v>
+        <v>1036</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>1044</v>
+        <v>1037</v>
       </c>
       <c r="Y55" s="1"/>
       <c r="Z55" s="1"/>
@@ -6095,18 +6109,18 @@
       <c r="AJ55" s="1"/>
       <c r="AK55" s="1"/>
     </row>
-    <row r="56" spans="1:37" ht="68" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:37" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>1045</v>
+        <v>1038</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1046</v>
+        <v>1039</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1047</v>
+        <v>1040</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>1048</v>
+        <v>1041</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>115</v>
@@ -6121,13 +6135,13 @@
         <v>474</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>1049</v>
+        <v>1042</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>1050</v>
+        <v>1043</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>1037</v>
+        <v>1044</v>
       </c>
       <c r="Y56" s="1"/>
       <c r="Z56" s="1"/>
@@ -6143,15 +6157,15 @@
       <c r="AJ56" s="1"/>
       <c r="AK56" s="1"/>
     </row>
-    <row r="57" spans="1:37" ht="51" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:37" ht="68" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>1051</v>
+        <v>1045</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1052</v>
+        <v>1046</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1053</v>
+        <v>1047</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>1048</v>
@@ -6169,13 +6183,13 @@
         <v>474</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>1054</v>
+        <v>1049</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>1055</v>
+        <v>1050</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>1056</v>
+        <v>1037</v>
       </c>
       <c r="Y57" s="1"/>
       <c r="Z57" s="1"/>
@@ -6193,13 +6207,13 @@
     </row>
     <row r="58" spans="1:37" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>1057</v>
+        <v>1051</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>1058</v>
+        <v>1052</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1059</v>
+        <v>1053</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>1048</v>
@@ -6217,13 +6231,13 @@
         <v>474</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>1060</v>
+        <v>1054</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>1061</v>
+        <v>1055</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>1062</v>
+        <v>1056</v>
       </c>
       <c r="Y58" s="1"/>
       <c r="Z58" s="1"/>
@@ -6241,13 +6255,13 @@
     </row>
     <row r="59" spans="1:37" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>1063</v>
+        <v>1057</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>1064</v>
+        <v>1058</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1065</v>
+        <v>1059</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>1048</v>
@@ -6265,10 +6279,13 @@
         <v>474</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>1066</v>
+        <v>1060</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>1067</v>
+        <v>1061</v>
+      </c>
+      <c r="Q59" s="1" t="s">
+        <v>1062</v>
       </c>
       <c r="Y59" s="1"/>
       <c r="Z59" s="1"/>
@@ -6286,13 +6303,13 @@
     </row>
     <row r="60" spans="1:37" ht="51" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>1068</v>
+        <v>1063</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>1052</v>
+        <v>1064</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>1048</v>
@@ -6310,10 +6327,10 @@
         <v>474</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
       <c r="Y60" s="1"/>
       <c r="Z60" s="1"/>
@@ -6331,13 +6348,13 @@
     </row>
     <row r="61" spans="1:37" ht="51" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>1052</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>1048</v>
@@ -6355,13 +6372,10 @@
         <v>474</v>
       </c>
       <c r="O61" s="1" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
       <c r="P61" s="1" t="s">
         <v>1071</v>
-      </c>
-      <c r="Q61" s="1" t="s">
-        <v>1056</v>
       </c>
       <c r="Y61" s="1"/>
       <c r="Z61" s="1"/>
@@ -6379,13 +6393,13 @@
     </row>
     <row r="62" spans="1:37" ht="51" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>1076</v>
+        <v>1052</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>1048</v>
@@ -6403,10 +6417,13 @@
         <v>474</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>1078</v>
+        <v>1074</v>
       </c>
       <c r="P62" s="1" t="s">
         <v>1071</v>
+      </c>
+      <c r="Q62" s="1" t="s">
+        <v>1056</v>
       </c>
       <c r="Y62" s="1"/>
       <c r="Z62" s="1"/>
@@ -6424,13 +6441,13 @@
     </row>
     <row r="63" spans="1:37" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>1079</v>
+        <v>1075</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>1052</v>
+        <v>1076</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>1048</v>
@@ -6448,13 +6465,10 @@
         <v>474</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="P63" s="1" t="s">
-        <v>1082</v>
-      </c>
-      <c r="Q63" s="1" t="s">
-        <v>1083</v>
+        <v>1071</v>
       </c>
       <c r="Y63" s="1"/>
       <c r="Z63" s="1"/>
@@ -6470,15 +6484,15 @@
       <c r="AJ63" s="1"/>
       <c r="AK63" s="1"/>
     </row>
-    <row r="64" spans="1:37" ht="102" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:37" ht="51" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>1084</v>
+        <v>1079</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>1052</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1085</v>
+        <v>1080</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>1048</v>
@@ -6496,13 +6510,13 @@
         <v>474</v>
       </c>
       <c r="O64" s="1" t="s">
-        <v>1086</v>
+        <v>1081</v>
       </c>
       <c r="P64" s="1" t="s">
-        <v>1087</v>
+        <v>1082</v>
       </c>
       <c r="Q64" s="1" t="s">
-        <v>1088</v>
+        <v>1083</v>
       </c>
       <c r="Y64" s="1"/>
       <c r="Z64" s="1"/>
@@ -6518,18 +6532,18 @@
       <c r="AJ64" s="1"/>
       <c r="AK64" s="1"/>
     </row>
-    <row r="65" spans="1:37" ht="51" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:37" ht="102" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>1090</v>
+        <v>1084</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>1052</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1091</v>
+        <v>1085</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>1092</v>
+        <v>1048</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>115</v>
@@ -6544,13 +6558,13 @@
         <v>474</v>
       </c>
       <c r="O65" s="1" t="s">
-        <v>1093</v>
-      </c>
-      <c r="P65" s="5" t="s">
-        <v>1094</v>
+        <v>1086</v>
+      </c>
+      <c r="P65" s="1" t="s">
+        <v>1087</v>
       </c>
       <c r="Q65" s="1" t="s">
-        <v>1095</v>
+        <v>1088</v>
       </c>
       <c r="Y65" s="1"/>
       <c r="Z65" s="1"/>
@@ -6566,18 +6580,18 @@
       <c r="AJ65" s="1"/>
       <c r="AK65" s="1"/>
     </row>
-    <row r="66" spans="1:37" ht="119" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:37" ht="51" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>1096</v>
+        <v>1090</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>1052</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1097</v>
+        <v>1091</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>1048</v>
+        <v>1092</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>115</v>
@@ -6592,13 +6606,13 @@
         <v>474</v>
       </c>
       <c r="O66" s="1" t="s">
-        <v>1098</v>
-      </c>
-      <c r="P66" s="1" t="s">
-        <v>1099</v>
+        <v>1093</v>
+      </c>
+      <c r="P66" s="5" t="s">
+        <v>1094</v>
       </c>
       <c r="Q66" s="1" t="s">
-        <v>1100</v>
+        <v>1095</v>
       </c>
       <c r="Y66" s="1"/>
       <c r="Z66" s="1"/>
@@ -6614,15 +6628,15 @@
       <c r="AJ66" s="1"/>
       <c r="AK66" s="1"/>
     </row>
-    <row r="67" spans="1:37" ht="51" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:37" ht="119" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>1101</v>
+        <v>1096</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>1052</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1102</v>
+        <v>1097</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>1048</v>
@@ -6640,13 +6654,13 @@
         <v>474</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>1103</v>
+        <v>1098</v>
       </c>
       <c r="P67" s="1" t="s">
-        <v>1104</v>
+        <v>1099</v>
       </c>
       <c r="Q67" s="1" t="s">
-        <v>1105</v>
+        <v>1100</v>
       </c>
       <c r="Y67" s="1"/>
       <c r="Z67" s="1"/>
@@ -6662,18 +6676,18 @@
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
     </row>
-    <row r="68" spans="1:37" ht="34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:37" ht="51" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>1106</v>
+        <v>1101</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>1107</v>
+        <v>1052</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1108</v>
+        <v>1102</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>1128</v>
+        <v>1048</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>115</v>
@@ -6688,13 +6702,13 @@
         <v>474</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>1109</v>
+        <v>1103</v>
       </c>
       <c r="P68" s="1" t="s">
-        <v>1110</v>
+        <v>1104</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>1111</v>
+        <v>1105</v>
       </c>
       <c r="Y68" s="1"/>
       <c r="Z68" s="1"/>
@@ -6710,18 +6724,18 @@
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
     </row>
-    <row r="69" spans="1:37" ht="51" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:37" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>1112</v>
+        <v>1106</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>1058</v>
+        <v>1107</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1113</v>
+        <v>1108</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1028</v>
+        <v>1128</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>115</v>
@@ -6736,13 +6750,13 @@
         <v>474</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>1114</v>
+        <v>1109</v>
       </c>
       <c r="P69" s="1" t="s">
-        <v>1115</v>
+        <v>1110</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>1116</v>
+        <v>1111</v>
       </c>
       <c r="Y69" s="1"/>
       <c r="Z69" s="1"/>
@@ -6758,18 +6772,18 @@
       <c r="AJ69" s="1"/>
       <c r="AK69" s="1"/>
     </row>
-    <row r="70" spans="1:37" ht="102" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:37" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>1117</v>
+        <v>1112</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>1058</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1118</v>
+        <v>1113</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>1048</v>
+        <v>1028</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>115</v>
@@ -6784,13 +6798,13 @@
         <v>474</v>
       </c>
       <c r="O70" s="1" t="s">
-        <v>1119</v>
+        <v>1114</v>
       </c>
       <c r="P70" s="1" t="s">
-        <v>1120</v>
+        <v>1115</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>1088</v>
+        <v>1116</v>
       </c>
       <c r="Y70" s="1"/>
       <c r="Z70" s="1"/>
@@ -6806,15 +6820,15 @@
       <c r="AJ70" s="1"/>
       <c r="AK70" s="1"/>
     </row>
-    <row r="71" spans="1:37" ht="119" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:37" ht="102" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>1058</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>1048</v>
@@ -6832,13 +6846,13 @@
         <v>474</v>
       </c>
       <c r="O71" s="1" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="P71" s="1" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
       <c r="Q71" s="1" t="s">
-        <v>1100</v>
+        <v>1088</v>
       </c>
       <c r="Y71" s="1"/>
       <c r="Z71" s="1"/>
@@ -6856,13 +6870,13 @@
     </row>
     <row r="72" spans="1:37" ht="119" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>1125</v>
+        <v>1121</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>1058</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>1048</v>
@@ -6880,10 +6894,10 @@
         <v>474</v>
       </c>
       <c r="O72" s="1" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="P72" s="1" t="s">
-        <v>1099</v>
+        <v>1124</v>
       </c>
       <c r="Q72" s="1" t="s">
         <v>1100</v>
@@ -6902,15 +6916,15 @@
       <c r="AJ72" s="1"/>
       <c r="AK72" s="1"/>
     </row>
-    <row r="73" spans="1:37" ht="102" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:37" ht="119" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>1137</v>
+        <v>1125</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>1026</v>
+        <v>1058</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1138</v>
+        <v>1126</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>1048</v>
@@ -6928,13 +6942,13 @@
         <v>474</v>
       </c>
       <c r="O73" s="1" t="s">
-        <v>1089</v>
+        <v>1127</v>
       </c>
       <c r="P73" s="1" t="s">
-        <v>1139</v>
+        <v>1099</v>
       </c>
       <c r="Q73" s="1" t="s">
-        <v>1088</v>
+        <v>1100</v>
       </c>
       <c r="Y73" s="1"/>
       <c r="Z73" s="1"/>
@@ -6950,18 +6964,18 @@
       <c r="AJ73" s="1"/>
       <c r="AK73" s="1"/>
     </row>
-    <row r="74" spans="1:37" ht="34" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:37" ht="102" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>1140</v>
+        <v>1137</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>1026</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1141</v>
+        <v>1138</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>1142</v>
+        <v>1048</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>115</v>
@@ -6979,7 +6993,10 @@
         <v>1089</v>
       </c>
       <c r="P74" s="1" t="s">
-        <v>1143</v>
+        <v>1139</v>
+      </c>
+      <c r="Q74" s="1" t="s">
+        <v>1088</v>
       </c>
       <c r="Y74" s="1"/>
       <c r="Z74" s="1"/>
@@ -6995,9 +7012,54 @@
       <c r="AJ74" s="1"/>
       <c r="AK74" s="1"/>
     </row>
+    <row r="75" spans="1:37" ht="34" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>1142</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="N75" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="O75" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="P75" s="1" t="s">
+        <v>1143</v>
+      </c>
+      <c r="Y75" s="1"/>
+      <c r="Z75" s="1"/>
+      <c r="AA75" s="1"/>
+      <c r="AB75" s="1"/>
+      <c r="AC75" s="1"/>
+      <c r="AD75" s="1"/>
+      <c r="AE75" s="1"/>
+      <c r="AF75" s="1"/>
+      <c r="AG75" s="1"/>
+      <c r="AH75" s="1"/>
+      <c r="AI75" s="1"/>
+      <c r="AJ75" s="1"/>
+      <c r="AK75" s="1"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AK51">
-    <sortCondition ref="A2:A51"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AK52">
+    <sortCondition ref="A2:A52"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update MODS for Green
</commit_message>
<xml_diff>
--- a/xml/OMV-MODS-worksheet.xlsx
+++ b/xml/OMV-MODS-worksheet.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/onemorevoice/xml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4AB51D-6EE6-B940-8817-D66C17A033C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC3E139-76AF-774D-8DBF-60FE77C26568}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="460" windowWidth="25020" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="25020" windowHeight="15260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
-    <sheet name="Artifacts" sheetId="1" r:id="rId2"/>
+    <sheet name="Visual Materials" sheetId="1" r:id="rId2"/>
     <sheet name="dev" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -3600,12 +3600,6 @@
 Sir Henry Morton Stanley; Dorothy (née Tennant), Lady Stanley; and 'Sali,' 1890</t>
   </si>
   <si>
-    <t>Interior with a Seated Man (Possibly an Agent for Elder Dempster or James Howie)</t>
-  </si>
-  <si>
-    <t>Interior with a Seated Man (Possibly an Agent for Elder Dempster or James Howie), [c.1892]</t>
-  </si>
-  <si>
     <t>Professional Wetstamp (Verso of Lose Print), [c.1895]</t>
   </si>
   <si>
@@ -3616,6 +3610,12 @@
   </si>
   <si>
     <t>Letter to [?] Phillips, 29 October 1868</t>
+  </si>
+  <si>
+    <t>Interior with a Seated Man (Possibly an Agent for Elder Dempster, Possibly James Howie)</t>
+  </si>
+  <si>
+    <t>Interior with a Seated Man (Possibly an Agent for Elder Dempster, Possibly James Howie), [c.1892]</t>
   </si>
 </sst>
 </file>
@@ -4105,7 +4105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
   <dimension ref="A1:AL77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
@@ -6315,10 +6315,10 @@
         <v>1038</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>1039</v>
@@ -7272,9 +7272,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ87"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G87" sqref="G87"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11041,10 +11041,10 @@
         <v>1168</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>1184</v>
+        <v>1188</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>1185</v>
+        <v>1189</v>
       </c>
       <c r="I86" s="7" t="s">
         <v>645</v>
@@ -11082,10 +11082,10 @@
         <v>1169</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="I87" s="7" t="s">
         <v>645</v>
@@ -11145,7 +11145,7 @@
         <v>413</v>
       </c>
       <c r="B1" t="str">
-        <f>Artifacts!I29</f>
+        <f>'Visual Materials'!I29</f>
         <v>Anonymous</v>
       </c>
       <c r="C1" t="s">
@@ -11155,14 +11155,14 @@
         <v>410</v>
       </c>
       <c r="E1" t="str">
-        <f>Artifacts!G29</f>
+        <f>'Visual Materials'!G29</f>
         <v>Pandita Ramabai Sarasvati</v>
       </c>
       <c r="F1" t="s">
         <v>412</v>
       </c>
       <c r="G1" t="str">
-        <f>Artifacts!S29</f>
+        <f>'Visual Materials'!S29</f>
         <v>[Late nineteenth century]</v>
       </c>
       <c r="H1" t="s">
@@ -11178,7 +11178,7 @@
         <v>413</v>
       </c>
       <c r="B2" t="str">
-        <f>Artifacts!I30</f>
+        <f>'Visual Materials'!I30</f>
         <v>J. Paul</v>
       </c>
       <c r="C2" t="s">
@@ -11188,14 +11188,14 @@
         <v>415</v>
       </c>
       <c r="E2" t="str">
-        <f>Artifacts!G30</f>
+        <f>'Visual Materials'!G30</f>
         <v>“Pandita Ramabai &amp; Her Gifted Daughter Manoramabai”</v>
       </c>
       <c r="F2" t="s">
         <v>412</v>
       </c>
       <c r="G2" t="str">
-        <f>Artifacts!S30</f>
+        <f>'Visual Materials'!S30</f>
         <v>[Early twentieth century]</v>
       </c>
       <c r="H2" t="s">
@@ -11211,7 +11211,7 @@
         <v>413</v>
       </c>
       <c r="B3" t="str">
-        <f>Artifacts!I31</f>
+        <f>'Visual Materials'!I31</f>
         <v>Anonymous</v>
       </c>
       <c r="C3" t="s">
@@ -11221,7 +11221,7 @@
         <v>416</v>
       </c>
       <c r="E3" t="str">
-        <f>Artifacts!G31</f>
+        <f>'Visual Materials'!G31</f>
         <v>E. Pauline Johnson</v>
       </c>
       <c r="F3" t="s">
@@ -11243,7 +11243,7 @@
         <v>413</v>
       </c>
       <c r="B4" t="str">
-        <f>Artifacts!I32</f>
+        <f>'Visual Materials'!I32</f>
         <v>Johnson, E. Pauline, 1861-1913</v>
       </c>
       <c r="C4" t="s">
@@ -11253,7 +11253,7 @@
         <v>417</v>
       </c>
       <c r="E4" t="str">
-        <f>Artifacts!G32</f>
+        <f>'Visual Materials'!G32</f>
         <v>“And He Said ‘Fight On’” (Manuscript Facsimile)</v>
       </c>
       <c r="F4" t="s">
@@ -11275,7 +11275,7 @@
         <v>413</v>
       </c>
       <c r="B5" t="str">
-        <f>Artifacts!I33</f>
+        <f>'Visual Materials'!I33</f>
         <v>Anonymous</v>
       </c>
       <c r="C5" t="s">
@@ -11285,7 +11285,7 @@
         <v>418</v>
       </c>
       <c r="E5" t="str">
-        <f>Artifacts!G33</f>
+        <f>'Visual Materials'!G33</f>
         <v>E. Pauline Johnson (with Facsimile Signature)</v>
       </c>
       <c r="F5" t="s">
@@ -11307,7 +11307,7 @@
         <v>413</v>
       </c>
       <c r="B6" t="str">
-        <f>Artifacts!I34</f>
+        <f>'Visual Materials'!I34</f>
         <v>Anonymous</v>
       </c>
       <c r="C6" t="s">
@@ -11317,7 +11317,7 @@
         <v>419</v>
       </c>
       <c r="E6" t="str">
-        <f>Artifacts!G34</f>
+        <f>'Visual Materials'!G34</f>
         <v>E. Pauline Johnson (with Facsimile Signature)</v>
       </c>
       <c r="F6" t="s">
@@ -11339,7 +11339,7 @@
         <v>413</v>
       </c>
       <c r="B7" t="str">
-        <f>Artifacts!I35</f>
+        <f>'Visual Materials'!I35</f>
         <v>Anonymous</v>
       </c>
       <c r="C7" t="s">
@@ -11349,7 +11349,7 @@
         <v>420</v>
       </c>
       <c r="E7" t="str">
-        <f>Artifacts!G35</f>
+        <f>'Visual Materials'!G35</f>
         <v>E. Pauline Johnson</v>
       </c>
       <c r="F7" t="s">
@@ -11371,7 +11371,7 @@
         <v>413</v>
       </c>
       <c r="B8" t="str">
-        <f>Artifacts!I36</f>
+        <f>'Visual Materials'!I36</f>
         <v>Anonymous</v>
       </c>
       <c r="C8" t="s">
@@ -11381,7 +11381,7 @@
         <v>421</v>
       </c>
       <c r="E8" t="str">
-        <f>Artifacts!G36</f>
+        <f>'Visual Materials'!G36</f>
         <v xml:space="preserve">“The Grave of Pauline Johnson in Stanley Park, Near Siwash Rock”; “Siwash Rock”; “The Spirit of Siwash Rock” </v>
       </c>
       <c r="F8" t="s">
@@ -11403,7 +11403,7 @@
         <v>413</v>
       </c>
       <c r="B9" t="str">
-        <f>Artifacts!I37</f>
+        <f>'Visual Materials'!I37</f>
         <v>Anonymous</v>
       </c>
       <c r="C9" t="s">
@@ -11413,7 +11413,7 @@
         <v>422</v>
       </c>
       <c r="E9" t="str">
-        <f>Artifacts!G37</f>
+        <f>'Visual Materials'!G37</f>
         <v>E. Pauline Johnson</v>
       </c>
       <c r="F9" t="s">

</xml_diff>

<commit_message>
update mods for tzatzoe
</commit_message>
<xml_diff>
--- a/xml/OMV-MODS-worksheet.xlsx
+++ b/xml/OMV-MODS-worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/onemorevoice/xml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F5A9AD-C649-764C-94A0-D028BE1D3B24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB667BC5-90DB-B24E-BF0E-8E97365C74F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="460" windowWidth="25020" windowHeight="15260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="25020" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2182" uniqueCount="1242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2204" uniqueCount="1252">
   <si>
     <t>liv_000017</t>
   </si>
@@ -3772,6 +3772,36 @@
   </si>
   <si>
     <t>liv_021004</t>
+  </si>
+  <si>
+    <t>liv_020025</t>
+  </si>
+  <si>
+    <t>liv_020026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CWM/LMS/South Africa/Incoming Correspondence/Box 16A/Folder 2/Jacket A </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CWM/LMS/South Africa/Incoming Correspondence/Box 21/Folder 3/Jacket B </t>
+  </si>
+  <si>
+    <t>1 September 1838</t>
+  </si>
+  <si>
+    <t>King Williams Town</t>
+  </si>
+  <si>
+    <t>8 October 1845</t>
+  </si>
+  <si>
+    <t>Letter to Directors of the London Missionary Society, 1 September 1838</t>
+  </si>
+  <si>
+    <t>Letter to Directors of the London Missionary Society, 8 October 1845</t>
+  </si>
+  <si>
+    <t>Letter to Directors of the London Missionary Society</t>
   </si>
 </sst>
 </file>
@@ -4259,11 +4289,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AL78"/>
+  <dimension ref="A1:AL80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7437,9 +7467,79 @@
       <c r="AK78" s="1"/>
       <c r="AL78" s="1"/>
     </row>
+    <row r="79" spans="1:38" ht="68" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N79" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O79" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P79" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="Q79" s="1" t="s">
+        <v>1246</v>
+      </c>
+      <c r="R79" s="1" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="80" spans="1:38" ht="68" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N80" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O80" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P80" s="1" t="s">
+        <v>1245</v>
+      </c>
+      <c r="Q80" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="R80" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AL53">
-    <sortCondition ref="A2:A53"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AL78">
+    <sortCondition ref="A2:A78"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7451,7 +7551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>

</xml_diff>